<commit_message>
Access Permissions Module completed with dynamic values
</commit_message>
<xml_diff>
--- a/src/test/resources/Utilites/Logindata.xlsx
+++ b/src/test/resources/Utilites/Logindata.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Backup\Projects\rhb.com\src\test\resources\Utilites\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Backup\Projects\RHB_Project\rhb.com\src\test\resources\Utilites\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1486A590-3D7D-4CC4-93BA-5DF573E68612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D00BFE1-4E5F-41D0-B512-EF9A70D5E8A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" r:id="rId1"/>
     <sheet name="Login_Test_Data" sheetId="2" r:id="rId2"/>
     <sheet name="Block_User" sheetId="3" r:id="rId3"/>
+    <sheet name="Access_Permission" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="39">
   <si>
     <t>Username</t>
   </si>
@@ -69,13 +70,88 @@
   </si>
   <si>
     <t xml:space="preserve">Your account has been disabled due to maximum failed login attempts. Please contact System Administrator. </t>
+  </si>
+  <si>
+    <t>Groups</t>
+  </si>
+  <si>
+    <t>GroupName</t>
+  </si>
+  <si>
+    <t>Group Description</t>
+  </si>
+  <si>
+    <t>Roles</t>
+  </si>
+  <si>
+    <t>Role Name</t>
+  </si>
+  <si>
+    <t>Super Admin</t>
+  </si>
+  <si>
+    <t>Select Group</t>
+  </si>
+  <si>
+    <t>Role Description</t>
+  </si>
+  <si>
+    <t>This is Group Description</t>
+  </si>
+  <si>
+    <t>This is Role Description</t>
+  </si>
+  <si>
+    <t>Users</t>
+  </si>
+  <si>
+    <t>LoginId</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>EmailId</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>User Fname</t>
+  </si>
+  <si>
+    <t>User Lname</t>
+  </si>
+  <si>
+    <t>test@gmail.com</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Groupssss</t>
+  </si>
+  <si>
+    <t>Rolessss</t>
+  </si>
+  <si>
+    <t>User2810</t>
+  </si>
+  <si>
+    <t>8881212888</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,6 +164,34 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -97,7 +201,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -105,15 +209,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -395,27 +525,28 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.08984375" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -429,7 +560,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection sqref="A1:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -441,56 +572,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -502,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42E7AA1D-5DFD-4641-879A-72DA977FD019}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -514,76 +646,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="8" t="s">
         <v>13</v>
       </c>
     </row>
@@ -591,4 +724,133 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D746129-08F1-4350-9A15-ED3449271664}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="22.26953125" customWidth="1"/>
+    <col min="2" max="2" width="31.453125" customWidth="1"/>
+    <col min="3" max="3" width="24.54296875" customWidth="1"/>
+    <col min="4" max="5" width="17.6328125" customWidth="1"/>
+    <col min="6" max="6" width="15.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="7"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D11" r:id="rId1" xr:uid="{C51F2DB2-B510-48FF-9793-67F30E0802B9}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modified the Whole project till Access Permissions module
</commit_message>
<xml_diff>
--- a/src/test/resources/Utilites/Logindata.xlsx
+++ b/src/test/resources/Utilites/Logindata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Backup\Projects\RHB_Project\rhb.com\src\test\resources\Utilites\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D00BFE1-4E5F-41D0-B512-EF9A70D5E8A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE44E05-85FF-401F-976F-BD8B12F25251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" r:id="rId1"/>
@@ -69,9 +69,6 @@
     <t>Check</t>
   </si>
   <si>
-    <t xml:space="preserve">Your account has been disabled due to maximum failed login attempts. Please contact System Administrator. </t>
-  </si>
-  <si>
     <t>Groups</t>
   </si>
   <si>
@@ -145,13 +142,16 @@
   </si>
   <si>
     <t>8881212888</t>
+  </si>
+  <si>
+    <t>Your account has been disabled due to maximum failed login attempts. Please contact System Administrator.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,6 +188,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -229,7 +235,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -237,10 +243,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -525,7 +532,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -546,12 +553,16 @@
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="9" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{40374208-B08C-4AB7-9B0D-C586AE90CCCD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -560,7 +571,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -634,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42E7AA1D-5DFD-4641-879A-72DA977FD019}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -716,8 +727,8 @@
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>13</v>
+      <c r="C7" s="7" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -730,8 +741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D746129-08F1-4350-9A15-ED3449271664}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView zoomScale="81" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -744,59 +755,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="7"/>
+      <c r="A1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="8"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -806,42 +817,42 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="F10" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified the ReadMe file with extra info
</commit_message>
<xml_diff>
--- a/src/test/resources/Utilites/Logindata.xlsx
+++ b/src/test/resources/Utilites/Logindata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Backup\Projects\RHB_Project\rhb.com\src\test\resources\Utilites\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE44E05-85FF-401F-976F-BD8B12F25251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB8DD4E7-A65F-4EFC-8504-1C3B1C2809F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -244,10 +244,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -553,7 +553,7 @@
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>3</v>
       </c>
     </row>
@@ -755,10 +755,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="8"/>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">

</xml_diff>